<commit_message>
Update sample data, templates, and application files
</commit_message>
<xml_diff>
--- a/assets/templates/Financial_Model_SAMPLE_DEMO_USD_thousands_GAAP.xlsx
+++ b/assets/templates/Financial_Model_SAMPLE_DEMO_USD_thousands_GAAP.xlsx
@@ -2070,7 +2070,7 @@
     <row r="15" outlineLevel="1" ht="14.5" customHeight="1">
       <c r="A15" s="14" t="inlineStr">
         <is>
-          <t>Depreciation (Percent of Sales)</t>
+          <t>D&amp;A % of Sales</t>
         </is>
       </c>
       <c r="B15" s="101">
@@ -2089,7 +2089,7 @@
     <row r="16" outlineLevel="1" ht="14.5" customHeight="1">
       <c r="A16" s="14" t="inlineStr">
         <is>
-          <t>Long Term Debt Interest (Average Debt)</t>
+          <t>LTD Rate (Avg Debt)</t>
         </is>
       </c>
       <c r="B16" s="101">
@@ -2108,7 +2108,7 @@
     <row r="17" outlineLevel="1" ht="14.5" customHeight="1">
       <c r="A17" s="14" t="inlineStr">
         <is>
-          <t>Tax Rate (Percent of EBT)</t>
+          <t>Tax Rate (Assumption)</t>
         </is>
       </c>
       <c r="B17" s="101">
@@ -2495,19 +2495,18 @@
           <t>Taxes</t>
         </is>
       </c>
-      <c r="B42" s="97">
-        <f>IF(B41&gt;0,B41*$B$8,0)</f>
-        <v/>
-      </c>
-      <c r="C42" s="97">
-        <f>IF(C41&gt;0,C41*$B$8,0)</f>
-        <v/>
-      </c>
-      <c r="D42" s="97">
-        <f>IF(D41&gt;0,D41*$B$8,0)</f>
-        <v/>
-      </c>
-      <c r="E42" s="17" t="n"/>
+      <c r="B42" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" outlineLevel="1" ht="14.5" customHeight="1" thickBot="1">
       <c r="A43" s="32" t="inlineStr">
@@ -2974,15 +2973,16 @@
         </is>
       </c>
       <c r="B77" s="105" t="n">
-        <v>73.10000000000002</v>
-      </c>
-      <c r="C77" s="97">
-        <f>B77+C43-C45</f>
-        <v/>
-      </c>
-      <c r="D77" s="97">
-        <f>C77+D43-D45</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C77" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="97" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78" outlineLevel="1" ht="14.5" customHeight="1">
@@ -3720,7 +3720,6 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
@@ -3735,7 +3734,6 @@
         </is>
       </c>
     </row>
-    <row r="8"/>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>

</xml_diff>